<commit_message>
update spreadsheet, modify program to read data from multiple worksheets
</commit_message>
<xml_diff>
--- a/soQuestion53446800.xlsx
+++ b/soQuestion53446800.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leona\gitrepos\stackoverflowanswers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D30026A5-5E61-4EC1-AB78-9EACC731E07B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DA9B2C6A-4BE1-446A-8EA0-EA9EB3DF89CE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10176" activeTab="2" xr2:uid="{2C6DBC11-9839-47B1-B62E-31AE914142D6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10176" activeTab="1" xr2:uid="{2C6DBC11-9839-47B1-B62E-31AE914142D6}"/>
   </bookViews>
   <sheets>
     <sheet name="2018" sheetId="1" r:id="rId1"/>
@@ -1522,8 +1522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47629CA7-3FE6-4A11-B6FC-F731421184EC}">
   <dimension ref="A2:AW9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AV5" sqref="AV5:AW9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1750,171 +1750,171 @@
       </c>
       <c r="B5">
         <f>SUM(E5,H5,K5)</f>
-        <v>2100</v>
+        <v>33000</v>
       </c>
       <c r="C5">
         <f t="shared" ref="C5:D9" si="0">SUM(F5,I5,L5)</f>
-        <v>900</v>
+        <v>15000</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>1200</v>
+        <v>18000</v>
       </c>
       <c r="E5">
         <f>SUM(F5:G5)</f>
-        <v>300</v>
+        <v>7000</v>
       </c>
       <c r="F5">
-        <v>100</v>
+        <v>3000</v>
       </c>
       <c r="G5">
-        <v>200</v>
+        <v>4000</v>
       </c>
       <c r="H5">
         <f>SUM(I5:J5)</f>
-        <v>700</v>
+        <v>11000</v>
       </c>
       <c r="I5">
-        <v>300</v>
+        <v>5000</v>
       </c>
       <c r="J5">
-        <v>400</v>
+        <v>6000</v>
       </c>
       <c r="K5">
         <f>SUM(L5:M5)</f>
-        <v>1100</v>
+        <v>15000</v>
       </c>
       <c r="L5">
-        <v>500</v>
+        <v>7000</v>
       </c>
       <c r="M5">
-        <v>600</v>
+        <v>8000</v>
       </c>
       <c r="N5">
         <f>SUM(Q5,T5,W5)</f>
-        <v>5100</v>
+        <v>69000</v>
       </c>
       <c r="O5">
         <f t="shared" ref="O5:P9" si="1">SUM(R5,U5,X5)</f>
-        <v>2400</v>
+        <v>33000</v>
       </c>
       <c r="P5">
         <f t="shared" si="1"/>
-        <v>2700</v>
+        <v>36000</v>
       </c>
       <c r="Q5">
         <f>SUM(R5:S5)</f>
-        <v>1300</v>
+        <v>19000</v>
       </c>
       <c r="R5">
-        <v>600</v>
+        <v>9000</v>
       </c>
       <c r="S5">
-        <v>700</v>
+        <v>10000</v>
       </c>
       <c r="T5">
         <f>SUM(U5:V5)</f>
-        <v>1700</v>
+        <v>23000</v>
       </c>
       <c r="U5">
-        <v>800</v>
+        <v>11000</v>
       </c>
       <c r="V5">
-        <v>900</v>
+        <v>12000</v>
       </c>
       <c r="W5">
         <f>SUM(X5:Y5)</f>
-        <v>2100</v>
+        <v>27000</v>
       </c>
       <c r="X5">
-        <v>1000</v>
+        <v>13000</v>
       </c>
       <c r="Y5">
-        <v>1100</v>
+        <v>14000</v>
       </c>
       <c r="Z5">
         <f>SUM(AC5,AF5,AI5)</f>
-        <v>8700</v>
+        <v>105000</v>
       </c>
       <c r="AA5">
         <f t="shared" ref="AA5:AB9" si="2">SUM(AD5,AG5,AJ5)</f>
-        <v>4200</v>
+        <v>51000</v>
       </c>
       <c r="AB5">
         <f t="shared" si="2"/>
-        <v>4500</v>
+        <v>54000</v>
       </c>
       <c r="AC5">
         <f>SUM(AD5:AE5)</f>
-        <v>2500</v>
+        <v>31000</v>
       </c>
       <c r="AD5">
-        <v>1200</v>
+        <v>15000</v>
       </c>
       <c r="AE5">
-        <v>1300</v>
+        <v>16000</v>
       </c>
       <c r="AF5">
         <f>SUM(AG5:AH5)</f>
-        <v>2900</v>
+        <v>35000</v>
       </c>
       <c r="AG5">
-        <v>1400</v>
+        <v>17000</v>
       </c>
       <c r="AH5">
-        <v>1500</v>
+        <v>18000</v>
       </c>
       <c r="AI5">
         <f>SUM(AJ5:AK5)</f>
-        <v>3300</v>
+        <v>39000</v>
       </c>
       <c r="AJ5">
-        <v>1600</v>
+        <v>19000</v>
       </c>
       <c r="AK5">
-        <v>1700</v>
+        <v>20000</v>
       </c>
       <c r="AL5">
         <f>SUM(AO5,AR5,AU5)</f>
-        <v>12900</v>
+        <v>141000</v>
       </c>
       <c r="AM5">
         <f t="shared" ref="AM5:AN9" si="3">SUM(AP5,AS5,AV5)</f>
-        <v>6300</v>
+        <v>69000</v>
       </c>
       <c r="AN5">
         <f t="shared" si="3"/>
-        <v>6600</v>
+        <v>72000</v>
       </c>
       <c r="AO5">
         <f>SUM(AP5:AQ5)</f>
-        <v>3900</v>
+        <v>43000</v>
       </c>
       <c r="AP5">
-        <v>1900</v>
+        <v>21000</v>
       </c>
       <c r="AQ5">
-        <v>2000</v>
+        <v>22000</v>
       </c>
       <c r="AR5">
         <f>SUM(AS5:AT5)</f>
-        <v>4300</v>
+        <v>47000</v>
       </c>
       <c r="AS5">
-        <v>2100</v>
+        <v>23000</v>
       </c>
       <c r="AT5">
-        <v>2200</v>
+        <v>24000</v>
       </c>
       <c r="AU5">
         <f>SUM(AV5:AW5)</f>
-        <v>4700</v>
+        <v>51000</v>
       </c>
       <c r="AV5">
-        <v>2300</v>
+        <v>25000</v>
       </c>
       <c r="AW5">
-        <v>2400</v>
+        <v>26000</v>
       </c>
     </row>
     <row r="6" spans="1:49" x14ac:dyDescent="0.3">
@@ -1923,171 +1923,171 @@
       </c>
       <c r="B6">
         <f t="shared" ref="B6:B9" si="4">SUM(E6,H6,K6)</f>
-        <v>2100</v>
+        <v>33000</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>15000</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>1200</v>
+        <v>18000</v>
       </c>
       <c r="E6">
         <f t="shared" ref="E6:E9" si="5">SUM(F6:G6)</f>
-        <v>300</v>
+        <v>7000</v>
       </c>
       <c r="F6">
-        <v>100</v>
+        <v>3000</v>
       </c>
       <c r="G6">
-        <v>200</v>
+        <v>4000</v>
       </c>
       <c r="H6">
         <f t="shared" ref="H6:H9" si="6">SUM(I6:J6)</f>
-        <v>700</v>
+        <v>11000</v>
       </c>
       <c r="I6">
-        <v>300</v>
+        <v>5000</v>
       </c>
       <c r="J6">
-        <v>400</v>
+        <v>6000</v>
       </c>
       <c r="K6">
         <f t="shared" ref="K6:K9" si="7">SUM(L6:M6)</f>
-        <v>1100</v>
+        <v>15000</v>
       </c>
       <c r="L6">
-        <v>500</v>
+        <v>7000</v>
       </c>
       <c r="M6">
-        <v>600</v>
+        <v>8000</v>
       </c>
       <c r="N6">
         <f t="shared" ref="N6:N9" si="8">SUM(Q6,T6,W6)</f>
-        <v>5100</v>
+        <v>69000</v>
       </c>
       <c r="O6">
         <f t="shared" si="1"/>
-        <v>2400</v>
+        <v>33000</v>
       </c>
       <c r="P6">
         <f t="shared" si="1"/>
-        <v>2700</v>
+        <v>36000</v>
       </c>
       <c r="Q6">
         <f t="shared" ref="Q6:Q9" si="9">SUM(R6:S6)</f>
-        <v>1300</v>
+        <v>19000</v>
       </c>
       <c r="R6">
-        <v>600</v>
+        <v>9000</v>
       </c>
       <c r="S6">
-        <v>700</v>
+        <v>10000</v>
       </c>
       <c r="T6">
         <f t="shared" ref="T6:T9" si="10">SUM(U6:V6)</f>
-        <v>1700</v>
+        <v>23000</v>
       </c>
       <c r="U6">
-        <v>800</v>
+        <v>11000</v>
       </c>
       <c r="V6">
-        <v>900</v>
+        <v>12000</v>
       </c>
       <c r="W6">
         <f t="shared" ref="W6:W9" si="11">SUM(X6:Y6)</f>
-        <v>2100</v>
+        <v>27000</v>
       </c>
       <c r="X6">
-        <v>1000</v>
+        <v>13000</v>
       </c>
       <c r="Y6">
-        <v>1100</v>
+        <v>14000</v>
       </c>
       <c r="Z6">
         <f t="shared" ref="Z6:Z9" si="12">SUM(AC6,AF6,AI6)</f>
-        <v>8700</v>
+        <v>105000</v>
       </c>
       <c r="AA6">
-        <f t="shared" si="2"/>
-        <v>4200</v>
+        <f t="shared" ref="AA6:AA9" si="13">SUM(AD6,AG6,AJ6)</f>
+        <v>51000</v>
       </c>
       <c r="AB6">
-        <f t="shared" si="2"/>
-        <v>4500</v>
+        <f t="shared" ref="AB6:AB9" si="14">SUM(AE6,AH6,AK6)</f>
+        <v>54000</v>
       </c>
       <c r="AC6">
-        <f t="shared" ref="AC6:AC9" si="13">SUM(AD6:AE6)</f>
-        <v>2500</v>
+        <f t="shared" ref="AC6:AC9" si="15">SUM(AD6:AE6)</f>
+        <v>31000</v>
       </c>
       <c r="AD6">
-        <v>1200</v>
+        <v>15000</v>
       </c>
       <c r="AE6">
-        <v>1300</v>
+        <v>16000</v>
       </c>
       <c r="AF6">
-        <f t="shared" ref="AF6:AF9" si="14">SUM(AG6:AH6)</f>
-        <v>2900</v>
+        <f t="shared" ref="AF6:AF9" si="16">SUM(AG6:AH6)</f>
+        <v>35000</v>
       </c>
       <c r="AG6">
-        <v>1400</v>
+        <v>17000</v>
       </c>
       <c r="AH6">
-        <v>1500</v>
+        <v>18000</v>
       </c>
       <c r="AI6">
-        <f t="shared" ref="AI6:AI9" si="15">SUM(AJ6:AK6)</f>
-        <v>3300</v>
+        <f t="shared" ref="AI6:AI9" si="17">SUM(AJ6:AK6)</f>
+        <v>39000</v>
       </c>
       <c r="AJ6">
-        <v>1600</v>
+        <v>19000</v>
       </c>
       <c r="AK6">
-        <v>1700</v>
+        <v>20000</v>
       </c>
       <c r="AL6">
-        <f t="shared" ref="AL6:AL9" si="16">SUM(AO6,AR6,AU6)</f>
-        <v>12900</v>
+        <f t="shared" ref="AL6:AL9" si="18">SUM(AO6,AR6,AU6)</f>
+        <v>141000</v>
       </c>
       <c r="AM6">
         <f t="shared" si="3"/>
-        <v>6300</v>
+        <v>69000</v>
       </c>
       <c r="AN6">
         <f t="shared" si="3"/>
-        <v>6600</v>
+        <v>72000</v>
       </c>
       <c r="AO6">
-        <f t="shared" ref="AO6:AO9" si="17">SUM(AP6:AQ6)</f>
-        <v>3900</v>
+        <f t="shared" ref="AO6:AO9" si="19">SUM(AP6:AQ6)</f>
+        <v>43000</v>
       </c>
       <c r="AP6">
-        <v>1900</v>
+        <v>21000</v>
       </c>
       <c r="AQ6">
-        <v>2000</v>
+        <v>22000</v>
       </c>
       <c r="AR6">
-        <f t="shared" ref="AR6:AR9" si="18">SUM(AS6:AT6)</f>
-        <v>4300</v>
+        <f t="shared" ref="AR6:AR9" si="20">SUM(AS6:AT6)</f>
+        <v>47000</v>
       </c>
       <c r="AS6">
-        <v>2100</v>
+        <v>23000</v>
       </c>
       <c r="AT6">
-        <v>2200</v>
+        <v>24000</v>
       </c>
       <c r="AU6">
-        <f t="shared" ref="AU6:AU9" si="19">SUM(AV6:AW6)</f>
-        <v>4700</v>
+        <f t="shared" ref="AU6:AU9" si="21">SUM(AV6:AW6)</f>
+        <v>51000</v>
       </c>
       <c r="AV6">
-        <v>2300</v>
+        <v>25000</v>
       </c>
       <c r="AW6">
-        <v>2400</v>
+        <v>26000</v>
       </c>
     </row>
     <row r="7" spans="1:49" x14ac:dyDescent="0.3">
@@ -2096,171 +2096,171 @@
       </c>
       <c r="B7">
         <f t="shared" si="4"/>
-        <v>2100</v>
+        <v>33000</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>15000</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>1200</v>
+        <v>18000</v>
       </c>
       <c r="E7">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>7000</v>
       </c>
       <c r="F7">
-        <v>100</v>
+        <v>3000</v>
       </c>
       <c r="G7">
-        <v>200</v>
+        <v>4000</v>
       </c>
       <c r="H7">
         <f t="shared" si="6"/>
-        <v>700</v>
+        <v>11000</v>
       </c>
       <c r="I7">
-        <v>300</v>
+        <v>5000</v>
       </c>
       <c r="J7">
-        <v>400</v>
+        <v>6000</v>
       </c>
       <c r="K7">
         <f t="shared" si="7"/>
-        <v>1100</v>
+        <v>15000</v>
       </c>
       <c r="L7">
-        <v>500</v>
+        <v>7000</v>
       </c>
       <c r="M7">
-        <v>600</v>
+        <v>8000</v>
       </c>
       <c r="N7">
         <f t="shared" si="8"/>
-        <v>5100</v>
+        <v>69000</v>
       </c>
       <c r="O7">
         <f t="shared" si="1"/>
-        <v>2400</v>
+        <v>33000</v>
       </c>
       <c r="P7">
         <f t="shared" si="1"/>
-        <v>2700</v>
+        <v>36000</v>
       </c>
       <c r="Q7">
         <f t="shared" si="9"/>
-        <v>1300</v>
+        <v>19000</v>
       </c>
       <c r="R7">
-        <v>600</v>
+        <v>9000</v>
       </c>
       <c r="S7">
-        <v>700</v>
+        <v>10000</v>
       </c>
       <c r="T7">
         <f t="shared" si="10"/>
-        <v>1700</v>
+        <v>23000</v>
       </c>
       <c r="U7">
-        <v>800</v>
+        <v>11000</v>
       </c>
       <c r="V7">
-        <v>900</v>
+        <v>12000</v>
       </c>
       <c r="W7">
         <f t="shared" si="11"/>
-        <v>2100</v>
+        <v>27000</v>
       </c>
       <c r="X7">
-        <v>1000</v>
+        <v>13000</v>
       </c>
       <c r="Y7">
-        <v>1100</v>
+        <v>14000</v>
       </c>
       <c r="Z7">
         <f t="shared" si="12"/>
-        <v>8700</v>
+        <v>105000</v>
       </c>
       <c r="AA7">
-        <f t="shared" si="2"/>
-        <v>4200</v>
+        <f t="shared" si="13"/>
+        <v>51000</v>
       </c>
       <c r="AB7">
-        <f t="shared" si="2"/>
-        <v>4500</v>
+        <f t="shared" si="14"/>
+        <v>54000</v>
       </c>
       <c r="AC7">
-        <f t="shared" si="13"/>
-        <v>2500</v>
+        <f t="shared" si="15"/>
+        <v>31000</v>
       </c>
       <c r="AD7">
-        <v>1200</v>
+        <v>15000</v>
       </c>
       <c r="AE7">
-        <v>1300</v>
+        <v>16000</v>
       </c>
       <c r="AF7">
-        <f t="shared" si="14"/>
-        <v>2900</v>
+        <f t="shared" si="16"/>
+        <v>35000</v>
       </c>
       <c r="AG7">
-        <v>1400</v>
+        <v>17000</v>
       </c>
       <c r="AH7">
-        <v>1500</v>
+        <v>18000</v>
       </c>
       <c r="AI7">
-        <f t="shared" si="15"/>
-        <v>3300</v>
+        <f t="shared" si="17"/>
+        <v>39000</v>
       </c>
       <c r="AJ7">
-        <v>1600</v>
+        <v>19000</v>
       </c>
       <c r="AK7">
-        <v>1700</v>
+        <v>20000</v>
       </c>
       <c r="AL7">
-        <f t="shared" si="16"/>
-        <v>12900</v>
+        <f t="shared" si="18"/>
+        <v>141000</v>
       </c>
       <c r="AM7">
         <f t="shared" si="3"/>
-        <v>6300</v>
+        <v>69000</v>
       </c>
       <c r="AN7">
         <f t="shared" si="3"/>
-        <v>6600</v>
+        <v>72000</v>
       </c>
       <c r="AO7">
-        <f t="shared" si="17"/>
-        <v>3900</v>
+        <f t="shared" si="19"/>
+        <v>43000</v>
       </c>
       <c r="AP7">
-        <v>1900</v>
+        <v>21000</v>
       </c>
       <c r="AQ7">
-        <v>2000</v>
+        <v>22000</v>
       </c>
       <c r="AR7">
-        <f t="shared" si="18"/>
-        <v>4300</v>
+        <f t="shared" si="20"/>
+        <v>47000</v>
       </c>
       <c r="AS7">
-        <v>2100</v>
+        <v>23000</v>
       </c>
       <c r="AT7">
-        <v>2200</v>
+        <v>24000</v>
       </c>
       <c r="AU7">
-        <f t="shared" si="19"/>
-        <v>4700</v>
+        <f t="shared" si="21"/>
+        <v>51000</v>
       </c>
       <c r="AV7">
-        <v>2300</v>
+        <v>25000</v>
       </c>
       <c r="AW7">
-        <v>2400</v>
+        <v>26000</v>
       </c>
     </row>
     <row r="8" spans="1:49" x14ac:dyDescent="0.3">
@@ -2269,171 +2269,171 @@
       </c>
       <c r="B8">
         <f t="shared" si="4"/>
-        <v>2100</v>
+        <v>33000</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>15000</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>1200</v>
+        <v>18000</v>
       </c>
       <c r="E8">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>7000</v>
       </c>
       <c r="F8">
-        <v>100</v>
+        <v>3000</v>
       </c>
       <c r="G8">
-        <v>200</v>
+        <v>4000</v>
       </c>
       <c r="H8">
         <f t="shared" si="6"/>
-        <v>700</v>
+        <v>11000</v>
       </c>
       <c r="I8">
-        <v>300</v>
+        <v>5000</v>
       </c>
       <c r="J8">
-        <v>400</v>
+        <v>6000</v>
       </c>
       <c r="K8">
         <f t="shared" si="7"/>
-        <v>1100</v>
+        <v>15000</v>
       </c>
       <c r="L8">
-        <v>500</v>
+        <v>7000</v>
       </c>
       <c r="M8">
-        <v>600</v>
+        <v>8000</v>
       </c>
       <c r="N8">
         <f t="shared" si="8"/>
-        <v>5100</v>
+        <v>69000</v>
       </c>
       <c r="O8">
         <f t="shared" si="1"/>
-        <v>2400</v>
+        <v>33000</v>
       </c>
       <c r="P8">
         <f t="shared" si="1"/>
-        <v>2700</v>
+        <v>36000</v>
       </c>
       <c r="Q8">
         <f t="shared" si="9"/>
-        <v>1300</v>
+        <v>19000</v>
       </c>
       <c r="R8">
-        <v>600</v>
+        <v>9000</v>
       </c>
       <c r="S8">
-        <v>700</v>
+        <v>10000</v>
       </c>
       <c r="T8">
         <f t="shared" si="10"/>
-        <v>1700</v>
+        <v>23000</v>
       </c>
       <c r="U8">
-        <v>800</v>
+        <v>11000</v>
       </c>
       <c r="V8">
-        <v>900</v>
+        <v>12000</v>
       </c>
       <c r="W8">
         <f t="shared" si="11"/>
-        <v>2100</v>
+        <v>27000</v>
       </c>
       <c r="X8">
-        <v>1000</v>
+        <v>13000</v>
       </c>
       <c r="Y8">
-        <v>1100</v>
+        <v>14000</v>
       </c>
       <c r="Z8">
         <f t="shared" si="12"/>
-        <v>8700</v>
+        <v>105000</v>
       </c>
       <c r="AA8">
-        <f t="shared" si="2"/>
-        <v>4200</v>
+        <f t="shared" si="13"/>
+        <v>51000</v>
       </c>
       <c r="AB8">
-        <f t="shared" si="2"/>
-        <v>4500</v>
+        <f t="shared" si="14"/>
+        <v>54000</v>
       </c>
       <c r="AC8">
-        <f t="shared" si="13"/>
-        <v>2500</v>
+        <f t="shared" si="15"/>
+        <v>31000</v>
       </c>
       <c r="AD8">
-        <v>1200</v>
+        <v>15000</v>
       </c>
       <c r="AE8">
-        <v>1300</v>
+        <v>16000</v>
       </c>
       <c r="AF8">
-        <f t="shared" si="14"/>
-        <v>2900</v>
+        <f t="shared" si="16"/>
+        <v>35000</v>
       </c>
       <c r="AG8">
-        <v>1400</v>
+        <v>17000</v>
       </c>
       <c r="AH8">
-        <v>1500</v>
+        <v>18000</v>
       </c>
       <c r="AI8">
-        <f t="shared" si="15"/>
-        <v>3300</v>
+        <f t="shared" si="17"/>
+        <v>39000</v>
       </c>
       <c r="AJ8">
-        <v>1600</v>
+        <v>19000</v>
       </c>
       <c r="AK8">
-        <v>1700</v>
+        <v>20000</v>
       </c>
       <c r="AL8">
-        <f t="shared" si="16"/>
-        <v>12900</v>
+        <f t="shared" si="18"/>
+        <v>141000</v>
       </c>
       <c r="AM8">
         <f t="shared" si="3"/>
-        <v>6300</v>
+        <v>69000</v>
       </c>
       <c r="AN8">
         <f t="shared" si="3"/>
-        <v>6600</v>
+        <v>72000</v>
       </c>
       <c r="AO8">
-        <f t="shared" si="17"/>
-        <v>3900</v>
+        <f t="shared" si="19"/>
+        <v>43000</v>
       </c>
       <c r="AP8">
-        <v>1900</v>
+        <v>21000</v>
       </c>
       <c r="AQ8">
-        <v>2000</v>
+        <v>22000</v>
       </c>
       <c r="AR8">
-        <f t="shared" si="18"/>
-        <v>4300</v>
+        <f t="shared" si="20"/>
+        <v>47000</v>
       </c>
       <c r="AS8">
-        <v>2100</v>
+        <v>23000</v>
       </c>
       <c r="AT8">
-        <v>2200</v>
+        <v>24000</v>
       </c>
       <c r="AU8">
-        <f t="shared" si="19"/>
-        <v>4700</v>
+        <f t="shared" si="21"/>
+        <v>51000</v>
       </c>
       <c r="AV8">
-        <v>2300</v>
+        <v>25000</v>
       </c>
       <c r="AW8">
-        <v>2400</v>
+        <v>26000</v>
       </c>
     </row>
     <row r="9" spans="1:49" x14ac:dyDescent="0.3">
@@ -2442,171 +2442,171 @@
       </c>
       <c r="B9">
         <f t="shared" si="4"/>
-        <v>2100</v>
+        <v>33000</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>15000</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>1200</v>
+        <v>18000</v>
       </c>
       <c r="E9">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>7000</v>
       </c>
       <c r="F9">
-        <v>100</v>
+        <v>3000</v>
       </c>
       <c r="G9">
-        <v>200</v>
+        <v>4000</v>
       </c>
       <c r="H9">
         <f t="shared" si="6"/>
-        <v>700</v>
+        <v>11000</v>
       </c>
       <c r="I9">
-        <v>300</v>
+        <v>5000</v>
       </c>
       <c r="J9">
-        <v>400</v>
+        <v>6000</v>
       </c>
       <c r="K9">
         <f t="shared" si="7"/>
-        <v>1100</v>
+        <v>15000</v>
       </c>
       <c r="L9">
-        <v>500</v>
+        <v>7000</v>
       </c>
       <c r="M9">
-        <v>600</v>
+        <v>8000</v>
       </c>
       <c r="N9">
         <f t="shared" si="8"/>
-        <v>5100</v>
+        <v>69000</v>
       </c>
       <c r="O9">
         <f t="shared" si="1"/>
-        <v>2400</v>
+        <v>33000</v>
       </c>
       <c r="P9">
         <f t="shared" si="1"/>
-        <v>2700</v>
+        <v>36000</v>
       </c>
       <c r="Q9">
         <f t="shared" si="9"/>
-        <v>1300</v>
+        <v>19000</v>
       </c>
       <c r="R9">
-        <v>600</v>
+        <v>9000</v>
       </c>
       <c r="S9">
-        <v>700</v>
+        <v>10000</v>
       </c>
       <c r="T9">
         <f t="shared" si="10"/>
-        <v>1700</v>
+        <v>23000</v>
       </c>
       <c r="U9">
-        <v>800</v>
+        <v>11000</v>
       </c>
       <c r="V9">
-        <v>900</v>
+        <v>12000</v>
       </c>
       <c r="W9">
         <f t="shared" si="11"/>
-        <v>2100</v>
+        <v>27000</v>
       </c>
       <c r="X9">
-        <v>1000</v>
+        <v>13000</v>
       </c>
       <c r="Y9">
-        <v>1100</v>
+        <v>14000</v>
       </c>
       <c r="Z9">
         <f t="shared" si="12"/>
-        <v>8700</v>
+        <v>105000</v>
       </c>
       <c r="AA9">
-        <f t="shared" si="2"/>
-        <v>4200</v>
+        <f t="shared" si="13"/>
+        <v>51000</v>
       </c>
       <c r="AB9">
-        <f t="shared" si="2"/>
-        <v>4500</v>
+        <f t="shared" si="14"/>
+        <v>54000</v>
       </c>
       <c r="AC9">
-        <f t="shared" si="13"/>
-        <v>2500</v>
+        <f t="shared" si="15"/>
+        <v>31000</v>
       </c>
       <c r="AD9">
-        <v>1200</v>
+        <v>15000</v>
       </c>
       <c r="AE9">
-        <v>1300</v>
+        <v>16000</v>
       </c>
       <c r="AF9">
-        <f t="shared" si="14"/>
-        <v>2900</v>
+        <f t="shared" si="16"/>
+        <v>35000</v>
       </c>
       <c r="AG9">
-        <v>1400</v>
+        <v>17000</v>
       </c>
       <c r="AH9">
-        <v>1500</v>
+        <v>18000</v>
       </c>
       <c r="AI9">
-        <f t="shared" si="15"/>
-        <v>3300</v>
+        <f t="shared" si="17"/>
+        <v>39000</v>
       </c>
       <c r="AJ9">
-        <v>1600</v>
+        <v>19000</v>
       </c>
       <c r="AK9">
-        <v>1700</v>
+        <v>20000</v>
       </c>
       <c r="AL9">
-        <f t="shared" si="16"/>
-        <v>12900</v>
+        <f t="shared" si="18"/>
+        <v>141000</v>
       </c>
       <c r="AM9">
         <f t="shared" si="3"/>
-        <v>6300</v>
+        <v>69000</v>
       </c>
       <c r="AN9">
         <f t="shared" si="3"/>
-        <v>6600</v>
+        <v>72000</v>
       </c>
       <c r="AO9">
-        <f t="shared" si="17"/>
-        <v>3900</v>
+        <f t="shared" si="19"/>
+        <v>43000</v>
       </c>
       <c r="AP9">
-        <v>1900</v>
+        <v>21000</v>
       </c>
       <c r="AQ9">
-        <v>2000</v>
+        <v>22000</v>
       </c>
       <c r="AR9">
-        <f t="shared" si="18"/>
-        <v>4300</v>
+        <f t="shared" si="20"/>
+        <v>47000</v>
       </c>
       <c r="AS9">
-        <v>2100</v>
+        <v>23000</v>
       </c>
       <c r="AT9">
-        <v>2200</v>
+        <v>24000</v>
       </c>
       <c r="AU9">
-        <f t="shared" si="19"/>
-        <v>4700</v>
+        <f t="shared" si="21"/>
+        <v>51000</v>
       </c>
       <c r="AV9">
-        <v>2300</v>
+        <v>25000</v>
       </c>
       <c r="AW9">
-        <v>2400</v>
+        <v>26000</v>
       </c>
     </row>
   </sheetData>
@@ -2618,8 +2618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B451AE-F362-46D4-BA39-97644DD24B6E}">
   <dimension ref="A2:AW9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AW9" sqref="AW9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
final version, reading multiple years
</commit_message>
<xml_diff>
--- a/soQuestion53446800.xlsx
+++ b/soQuestion53446800.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leona\gitrepos\stackoverflowanswers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DA9B2C6A-4BE1-446A-8EA0-EA9EB3DF89CE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BF208286-E967-4A8C-9499-9DDE534C5FCD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10176" activeTab="1" xr2:uid="{2C6DBC11-9839-47B1-B62E-31AE914142D6}"/>
   </bookViews>
   <sheets>
     <sheet name="2018" sheetId="1" r:id="rId1"/>
     <sheet name="2017" sheetId="2" r:id="rId2"/>
-    <sheet name="2016" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="15">
   <si>
     <t>Country</t>
   </si>
@@ -427,7 +426,7 @@
   <dimension ref="A2:AW9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1522,7 +1521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47629CA7-3FE6-4A11-B6FC-F731421184EC}">
   <dimension ref="A2:AW9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AV5" sqref="AV5:AW9"/>
     </sheetView>
   </sheetViews>
@@ -2612,1100 +2611,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B451AE-F362-46D4-BA39-97644DD24B6E}">
-  <dimension ref="A2:AW9"/>
-  <sheetViews>
-    <sheetView topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AW9" sqref="AW9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" t="s">
-        <v>10</v>
-      </c>
-      <c r="O3" t="s">
-        <v>1</v>
-      </c>
-      <c r="R3" t="s">
-        <v>4</v>
-      </c>
-      <c r="U3" t="s">
-        <v>9</v>
-      </c>
-      <c r="X3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>4</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K4" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" t="s">
-        <v>2</v>
-      </c>
-      <c r="M4" t="s">
-        <v>3</v>
-      </c>
-      <c r="N4" t="s">
-        <v>1</v>
-      </c>
-      <c r="O4" t="s">
-        <v>2</v>
-      </c>
-      <c r="P4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>1</v>
-      </c>
-      <c r="R4" t="s">
-        <v>2</v>
-      </c>
-      <c r="S4" t="s">
-        <v>3</v>
-      </c>
-      <c r="T4" t="s">
-        <v>1</v>
-      </c>
-      <c r="U4" t="s">
-        <v>2</v>
-      </c>
-      <c r="V4" t="s">
-        <v>3</v>
-      </c>
-      <c r="W4" t="s">
-        <v>1</v>
-      </c>
-      <c r="X4" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <f>SUM(E5,H5,K5)</f>
-        <v>2100</v>
-      </c>
-      <c r="C5">
-        <f t="shared" ref="C5:D9" si="0">SUM(F5,I5,L5)</f>
-        <v>900</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>1200</v>
-      </c>
-      <c r="E5">
-        <f>SUM(F5:G5)</f>
-        <v>300</v>
-      </c>
-      <c r="F5">
-        <v>100</v>
-      </c>
-      <c r="G5">
-        <v>200</v>
-      </c>
-      <c r="H5">
-        <f>SUM(I5:J5)</f>
-        <v>700</v>
-      </c>
-      <c r="I5">
-        <v>300</v>
-      </c>
-      <c r="J5">
-        <v>400</v>
-      </c>
-      <c r="K5">
-        <f>SUM(L5:M5)</f>
-        <v>1100</v>
-      </c>
-      <c r="L5">
-        <v>500</v>
-      </c>
-      <c r="M5">
-        <v>600</v>
-      </c>
-      <c r="N5">
-        <f>SUM(Q5,T5,W5)</f>
-        <v>5100</v>
-      </c>
-      <c r="O5">
-        <f t="shared" ref="O5:P9" si="1">SUM(R5,U5,X5)</f>
-        <v>2400</v>
-      </c>
-      <c r="P5">
-        <f t="shared" si="1"/>
-        <v>2700</v>
-      </c>
-      <c r="Q5">
-        <f>SUM(R5:S5)</f>
-        <v>1300</v>
-      </c>
-      <c r="R5">
-        <v>600</v>
-      </c>
-      <c r="S5">
-        <v>700</v>
-      </c>
-      <c r="T5">
-        <f>SUM(U5:V5)</f>
-        <v>1700</v>
-      </c>
-      <c r="U5">
-        <v>800</v>
-      </c>
-      <c r="V5">
-        <v>900</v>
-      </c>
-      <c r="W5">
-        <f>SUM(X5:Y5)</f>
-        <v>2100</v>
-      </c>
-      <c r="X5">
-        <v>1000</v>
-      </c>
-      <c r="Y5">
-        <v>1100</v>
-      </c>
-      <c r="Z5">
-        <f>SUM(AC5,AF5,AI5)</f>
-        <v>8700</v>
-      </c>
-      <c r="AA5">
-        <f t="shared" ref="AA5:AB9" si="2">SUM(AD5,AG5,AJ5)</f>
-        <v>4200</v>
-      </c>
-      <c r="AB5">
-        <f t="shared" si="2"/>
-        <v>4500</v>
-      </c>
-      <c r="AC5">
-        <f>SUM(AD5:AE5)</f>
-        <v>2500</v>
-      </c>
-      <c r="AD5">
-        <v>1200</v>
-      </c>
-      <c r="AE5">
-        <v>1300</v>
-      </c>
-      <c r="AF5">
-        <f>SUM(AG5:AH5)</f>
-        <v>2900</v>
-      </c>
-      <c r="AG5">
-        <v>1400</v>
-      </c>
-      <c r="AH5">
-        <v>1500</v>
-      </c>
-      <c r="AI5">
-        <f>SUM(AJ5:AK5)</f>
-        <v>3300</v>
-      </c>
-      <c r="AJ5">
-        <v>1600</v>
-      </c>
-      <c r="AK5">
-        <v>1700</v>
-      </c>
-      <c r="AL5">
-        <f>SUM(AO5,AR5,AU5)</f>
-        <v>12900</v>
-      </c>
-      <c r="AM5">
-        <f t="shared" ref="AM5:AN9" si="3">SUM(AP5,AS5,AV5)</f>
-        <v>6300</v>
-      </c>
-      <c r="AN5">
-        <f t="shared" si="3"/>
-        <v>6600</v>
-      </c>
-      <c r="AO5">
-        <f>SUM(AP5:AQ5)</f>
-        <v>3900</v>
-      </c>
-      <c r="AP5">
-        <v>1900</v>
-      </c>
-      <c r="AQ5">
-        <v>2000</v>
-      </c>
-      <c r="AR5">
-        <f>SUM(AS5:AT5)</f>
-        <v>4300</v>
-      </c>
-      <c r="AS5">
-        <v>2100</v>
-      </c>
-      <c r="AT5">
-        <v>2200</v>
-      </c>
-      <c r="AU5">
-        <f>SUM(AV5:AW5)</f>
-        <v>4700</v>
-      </c>
-      <c r="AV5">
-        <v>2300</v>
-      </c>
-      <c r="AW5">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <f t="shared" ref="B6:B9" si="4">SUM(E6,H6,K6)</f>
-        <v>2100</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>900</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>1200</v>
-      </c>
-      <c r="E6">
-        <f t="shared" ref="E6:E9" si="5">SUM(F6:G6)</f>
-        <v>300</v>
-      </c>
-      <c r="F6">
-        <v>100</v>
-      </c>
-      <c r="G6">
-        <v>200</v>
-      </c>
-      <c r="H6">
-        <f t="shared" ref="H6:H9" si="6">SUM(I6:J6)</f>
-        <v>700</v>
-      </c>
-      <c r="I6">
-        <v>300</v>
-      </c>
-      <c r="J6">
-        <v>400</v>
-      </c>
-      <c r="K6">
-        <f t="shared" ref="K6:K9" si="7">SUM(L6:M6)</f>
-        <v>1100</v>
-      </c>
-      <c r="L6">
-        <v>500</v>
-      </c>
-      <c r="M6">
-        <v>600</v>
-      </c>
-      <c r="N6">
-        <f t="shared" ref="N6:N9" si="8">SUM(Q6,T6,W6)</f>
-        <v>5100</v>
-      </c>
-      <c r="O6">
-        <f t="shared" si="1"/>
-        <v>2400</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="1"/>
-        <v>2700</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" ref="Q6:Q9" si="9">SUM(R6:S6)</f>
-        <v>1300</v>
-      </c>
-      <c r="R6">
-        <v>600</v>
-      </c>
-      <c r="S6">
-        <v>700</v>
-      </c>
-      <c r="T6">
-        <f t="shared" ref="T6:T9" si="10">SUM(U6:V6)</f>
-        <v>1700</v>
-      </c>
-      <c r="U6">
-        <v>800</v>
-      </c>
-      <c r="V6">
-        <v>900</v>
-      </c>
-      <c r="W6">
-        <f t="shared" ref="W6:W9" si="11">SUM(X6:Y6)</f>
-        <v>2100</v>
-      </c>
-      <c r="X6">
-        <v>1000</v>
-      </c>
-      <c r="Y6">
-        <v>1100</v>
-      </c>
-      <c r="Z6">
-        <f t="shared" ref="Z6:Z9" si="12">SUM(AC6,AF6,AI6)</f>
-        <v>8700</v>
-      </c>
-      <c r="AA6">
-        <f t="shared" si="2"/>
-        <v>4200</v>
-      </c>
-      <c r="AB6">
-        <f t="shared" si="2"/>
-        <v>4500</v>
-      </c>
-      <c r="AC6">
-        <f t="shared" ref="AC6:AC9" si="13">SUM(AD6:AE6)</f>
-        <v>2500</v>
-      </c>
-      <c r="AD6">
-        <v>1200</v>
-      </c>
-      <c r="AE6">
-        <v>1300</v>
-      </c>
-      <c r="AF6">
-        <f t="shared" ref="AF6:AF9" si="14">SUM(AG6:AH6)</f>
-        <v>2900</v>
-      </c>
-      <c r="AG6">
-        <v>1400</v>
-      </c>
-      <c r="AH6">
-        <v>1500</v>
-      </c>
-      <c r="AI6">
-        <f t="shared" ref="AI6:AI9" si="15">SUM(AJ6:AK6)</f>
-        <v>3300</v>
-      </c>
-      <c r="AJ6">
-        <v>1600</v>
-      </c>
-      <c r="AK6">
-        <v>1700</v>
-      </c>
-      <c r="AL6">
-        <f t="shared" ref="AL6:AL9" si="16">SUM(AO6,AR6,AU6)</f>
-        <v>12900</v>
-      </c>
-      <c r="AM6">
-        <f t="shared" si="3"/>
-        <v>6300</v>
-      </c>
-      <c r="AN6">
-        <f t="shared" si="3"/>
-        <v>6600</v>
-      </c>
-      <c r="AO6">
-        <f t="shared" ref="AO6:AO9" si="17">SUM(AP6:AQ6)</f>
-        <v>3900</v>
-      </c>
-      <c r="AP6">
-        <v>1900</v>
-      </c>
-      <c r="AQ6">
-        <v>2000</v>
-      </c>
-      <c r="AR6">
-        <f t="shared" ref="AR6:AR9" si="18">SUM(AS6:AT6)</f>
-        <v>4300</v>
-      </c>
-      <c r="AS6">
-        <v>2100</v>
-      </c>
-      <c r="AT6">
-        <v>2200</v>
-      </c>
-      <c r="AU6">
-        <f t="shared" ref="AU6:AU9" si="19">SUM(AV6:AW6)</f>
-        <v>4700</v>
-      </c>
-      <c r="AV6">
-        <v>2300</v>
-      </c>
-      <c r="AW6">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="4"/>
-        <v>2100</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>900</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>1200</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="5"/>
-        <v>300</v>
-      </c>
-      <c r="F7">
-        <v>100</v>
-      </c>
-      <c r="G7">
-        <v>200</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="6"/>
-        <v>700</v>
-      </c>
-      <c r="I7">
-        <v>300</v>
-      </c>
-      <c r="J7">
-        <v>400</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="7"/>
-        <v>1100</v>
-      </c>
-      <c r="L7">
-        <v>500</v>
-      </c>
-      <c r="M7">
-        <v>600</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="8"/>
-        <v>5100</v>
-      </c>
-      <c r="O7">
-        <f t="shared" si="1"/>
-        <v>2400</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="1"/>
-        <v>2700</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" si="9"/>
-        <v>1300</v>
-      </c>
-      <c r="R7">
-        <v>600</v>
-      </c>
-      <c r="S7">
-        <v>700</v>
-      </c>
-      <c r="T7">
-        <f t="shared" si="10"/>
-        <v>1700</v>
-      </c>
-      <c r="U7">
-        <v>800</v>
-      </c>
-      <c r="V7">
-        <v>900</v>
-      </c>
-      <c r="W7">
-        <f t="shared" si="11"/>
-        <v>2100</v>
-      </c>
-      <c r="X7">
-        <v>1000</v>
-      </c>
-      <c r="Y7">
-        <v>1100</v>
-      </c>
-      <c r="Z7">
-        <f t="shared" si="12"/>
-        <v>8700</v>
-      </c>
-      <c r="AA7">
-        <f t="shared" si="2"/>
-        <v>4200</v>
-      </c>
-      <c r="AB7">
-        <f t="shared" si="2"/>
-        <v>4500</v>
-      </c>
-      <c r="AC7">
-        <f t="shared" si="13"/>
-        <v>2500</v>
-      </c>
-      <c r="AD7">
-        <v>1200</v>
-      </c>
-      <c r="AE7">
-        <v>1300</v>
-      </c>
-      <c r="AF7">
-        <f t="shared" si="14"/>
-        <v>2900</v>
-      </c>
-      <c r="AG7">
-        <v>1400</v>
-      </c>
-      <c r="AH7">
-        <v>1500</v>
-      </c>
-      <c r="AI7">
-        <f t="shared" si="15"/>
-        <v>3300</v>
-      </c>
-      <c r="AJ7">
-        <v>1600</v>
-      </c>
-      <c r="AK7">
-        <v>1700</v>
-      </c>
-      <c r="AL7">
-        <f t="shared" si="16"/>
-        <v>12900</v>
-      </c>
-      <c r="AM7">
-        <f t="shared" si="3"/>
-        <v>6300</v>
-      </c>
-      <c r="AN7">
-        <f t="shared" si="3"/>
-        <v>6600</v>
-      </c>
-      <c r="AO7">
-        <f t="shared" si="17"/>
-        <v>3900</v>
-      </c>
-      <c r="AP7">
-        <v>1900</v>
-      </c>
-      <c r="AQ7">
-        <v>2000</v>
-      </c>
-      <c r="AR7">
-        <f t="shared" si="18"/>
-        <v>4300</v>
-      </c>
-      <c r="AS7">
-        <v>2100</v>
-      </c>
-      <c r="AT7">
-        <v>2200</v>
-      </c>
-      <c r="AU7">
-        <f t="shared" si="19"/>
-        <v>4700</v>
-      </c>
-      <c r="AV7">
-        <v>2300</v>
-      </c>
-      <c r="AW7">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="4"/>
-        <v>2100</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>900</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>1200</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="5"/>
-        <v>300</v>
-      </c>
-      <c r="F8">
-        <v>100</v>
-      </c>
-      <c r="G8">
-        <v>200</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="6"/>
-        <v>700</v>
-      </c>
-      <c r="I8">
-        <v>300</v>
-      </c>
-      <c r="J8">
-        <v>400</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="7"/>
-        <v>1100</v>
-      </c>
-      <c r="L8">
-        <v>500</v>
-      </c>
-      <c r="M8">
-        <v>600</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="8"/>
-        <v>5100</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="1"/>
-        <v>2400</v>
-      </c>
-      <c r="P8">
-        <f t="shared" si="1"/>
-        <v>2700</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="9"/>
-        <v>1300</v>
-      </c>
-      <c r="R8">
-        <v>600</v>
-      </c>
-      <c r="S8">
-        <v>700</v>
-      </c>
-      <c r="T8">
-        <f t="shared" si="10"/>
-        <v>1700</v>
-      </c>
-      <c r="U8">
-        <v>800</v>
-      </c>
-      <c r="V8">
-        <v>900</v>
-      </c>
-      <c r="W8">
-        <f t="shared" si="11"/>
-        <v>2100</v>
-      </c>
-      <c r="X8">
-        <v>1000</v>
-      </c>
-      <c r="Y8">
-        <v>1100</v>
-      </c>
-      <c r="Z8">
-        <f t="shared" si="12"/>
-        <v>8700</v>
-      </c>
-      <c r="AA8">
-        <f t="shared" si="2"/>
-        <v>4200</v>
-      </c>
-      <c r="AB8">
-        <f t="shared" si="2"/>
-        <v>4500</v>
-      </c>
-      <c r="AC8">
-        <f t="shared" si="13"/>
-        <v>2500</v>
-      </c>
-      <c r="AD8">
-        <v>1200</v>
-      </c>
-      <c r="AE8">
-        <v>1300</v>
-      </c>
-      <c r="AF8">
-        <f t="shared" si="14"/>
-        <v>2900</v>
-      </c>
-      <c r="AG8">
-        <v>1400</v>
-      </c>
-      <c r="AH8">
-        <v>1500</v>
-      </c>
-      <c r="AI8">
-        <f t="shared" si="15"/>
-        <v>3300</v>
-      </c>
-      <c r="AJ8">
-        <v>1600</v>
-      </c>
-      <c r="AK8">
-        <v>1700</v>
-      </c>
-      <c r="AL8">
-        <f t="shared" si="16"/>
-        <v>12900</v>
-      </c>
-      <c r="AM8">
-        <f t="shared" si="3"/>
-        <v>6300</v>
-      </c>
-      <c r="AN8">
-        <f t="shared" si="3"/>
-        <v>6600</v>
-      </c>
-      <c r="AO8">
-        <f t="shared" si="17"/>
-        <v>3900</v>
-      </c>
-      <c r="AP8">
-        <v>1900</v>
-      </c>
-      <c r="AQ8">
-        <v>2000</v>
-      </c>
-      <c r="AR8">
-        <f t="shared" si="18"/>
-        <v>4300</v>
-      </c>
-      <c r="AS8">
-        <v>2100</v>
-      </c>
-      <c r="AT8">
-        <v>2200</v>
-      </c>
-      <c r="AU8">
-        <f t="shared" si="19"/>
-        <v>4700</v>
-      </c>
-      <c r="AV8">
-        <v>2300</v>
-      </c>
-      <c r="AW8">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <f t="shared" si="4"/>
-        <v>2100</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>900</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>1200</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="5"/>
-        <v>300</v>
-      </c>
-      <c r="F9">
-        <v>100</v>
-      </c>
-      <c r="G9">
-        <v>200</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="6"/>
-        <v>700</v>
-      </c>
-      <c r="I9">
-        <v>300</v>
-      </c>
-      <c r="J9">
-        <v>400</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="7"/>
-        <v>1100</v>
-      </c>
-      <c r="L9">
-        <v>500</v>
-      </c>
-      <c r="M9">
-        <v>600</v>
-      </c>
-      <c r="N9">
-        <f t="shared" si="8"/>
-        <v>5100</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="1"/>
-        <v>2400</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="1"/>
-        <v>2700</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="9"/>
-        <v>1300</v>
-      </c>
-      <c r="R9">
-        <v>600</v>
-      </c>
-      <c r="S9">
-        <v>700</v>
-      </c>
-      <c r="T9">
-        <f t="shared" si="10"/>
-        <v>1700</v>
-      </c>
-      <c r="U9">
-        <v>800</v>
-      </c>
-      <c r="V9">
-        <v>900</v>
-      </c>
-      <c r="W9">
-        <f t="shared" si="11"/>
-        <v>2100</v>
-      </c>
-      <c r="X9">
-        <v>1000</v>
-      </c>
-      <c r="Y9">
-        <v>1100</v>
-      </c>
-      <c r="Z9">
-        <f t="shared" si="12"/>
-        <v>8700</v>
-      </c>
-      <c r="AA9">
-        <f t="shared" si="2"/>
-        <v>4200</v>
-      </c>
-      <c r="AB9">
-        <f t="shared" si="2"/>
-        <v>4500</v>
-      </c>
-      <c r="AC9">
-        <f t="shared" si="13"/>
-        <v>2500</v>
-      </c>
-      <c r="AD9">
-        <v>1200</v>
-      </c>
-      <c r="AE9">
-        <v>1300</v>
-      </c>
-      <c r="AF9">
-        <f t="shared" si="14"/>
-        <v>2900</v>
-      </c>
-      <c r="AG9">
-        <v>1400</v>
-      </c>
-      <c r="AH9">
-        <v>1500</v>
-      </c>
-      <c r="AI9">
-        <f t="shared" si="15"/>
-        <v>3300</v>
-      </c>
-      <c r="AJ9">
-        <v>1600</v>
-      </c>
-      <c r="AK9">
-        <v>1700</v>
-      </c>
-      <c r="AL9">
-        <f t="shared" si="16"/>
-        <v>12900</v>
-      </c>
-      <c r="AM9">
-        <f t="shared" si="3"/>
-        <v>6300</v>
-      </c>
-      <c r="AN9">
-        <f t="shared" si="3"/>
-        <v>6600</v>
-      </c>
-      <c r="AO9">
-        <f t="shared" si="17"/>
-        <v>3900</v>
-      </c>
-      <c r="AP9">
-        <v>1900</v>
-      </c>
-      <c r="AQ9">
-        <v>2000</v>
-      </c>
-      <c r="AR9">
-        <f t="shared" si="18"/>
-        <v>4300</v>
-      </c>
-      <c r="AS9">
-        <v>2100</v>
-      </c>
-      <c r="AT9">
-        <v>2200</v>
-      </c>
-      <c r="AU9">
-        <f t="shared" si="19"/>
-        <v>4700</v>
-      </c>
-      <c r="AV9">
-        <v>2300</v>
-      </c>
-      <c r="AW9">
-        <v>2400</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>